<commit_message>
ultimo layout tibrado sa
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/timbrado_tmm_q.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/timbrado_tmm_q.xlsx
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
   <si>
     <t>No. Empleado</t>
   </si>
@@ -516,7 +516,25 @@
     <t>Vales de despensa</t>
   </si>
   <si>
-    <t>NS</t>
+    <t>Deducciones</t>
+  </si>
+  <si>
+    <t>Comprobacion</t>
+  </si>
+  <si>
+    <t>NETO</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
+  <si>
+    <t>VALES</t>
+  </si>
+  <si>
+    <t>DIF</t>
   </si>
 </sst>
 </file>
@@ -896,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -926,7 +944,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -935,7 +952,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -957,24 +979,25 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1285,7 +1308,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD38"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,13 +2141,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:AO5"/>
+  <dimension ref="A1:AN5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AE25" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD103"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,14 +2155,15 @@
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
     <col min="3" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="12" width="9.140625"/>
+    <col min="9" max="11" width="9.140625"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
     <col min="13" max="24" width="9.140625" customWidth="1"/>
     <col min="25" max="28" width="9.85546875" customWidth="1"/>
     <col min="29" max="30" width="9.140625"/>
     <col min="31" max="35" width="9.85546875" customWidth="1"/>
     <col min="36" max="36" width="20" customWidth="1"/>
     <col min="37" max="40" width="9.85546875" customWidth="1"/>
-    <col min="41" max="41" width="10.5703125" style="23" customWidth="1"/>
+    <col min="41" max="41" width="10.5703125" customWidth="1"/>
     <col min="42" max="42" width="9.85546875" customWidth="1"/>
     <col min="43" max="43" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2238,18 +2262,18 @@
       <c r="M2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
       <c r="R2" s="35"/>
       <c r="S2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
       <c r="X2" s="33"/>
       <c r="Y2" s="34" t="s">
         <v>40</v>
@@ -2259,10 +2283,10 @@
         <v>41</v>
       </c>
       <c r="AB2" s="33"/>
-      <c r="AC2" s="38" t="s">
+      <c r="AC2" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AD2" s="39"/>
+      <c r="AD2" s="37"/>
       <c r="AE2" s="34" t="s">
         <v>42</v>
       </c>
@@ -2407,15 +2431,22 @@
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="S2:X2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="AM2:AN2"/>
     <mergeCell ref="Y2:Z2"/>
@@ -2424,13 +2455,6 @@
     <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="S2:X2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup scale="75" orientation="landscape" r:id="rId1"/>
@@ -2441,14 +2465,14 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:U248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="B44" sqref="B44"/>
       <selection pane="topRight" activeCell="B44" sqref="B44"/>
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD47"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,12 +2491,11 @@
     <col min="12" max="12" width="16.5703125" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="27" customWidth="1"/>
-    <col min="16" max="23" width="10.5703125" style="28" customWidth="1"/>
-    <col min="24" max="24" width="9.5703125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="26" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C1" s="17" t="s">
         <v>53</v>
       </c>
@@ -2509,46 +2532,48 @@
       <c r="N1" s="18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="40" t="s">
+      <c r="O1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C2" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="28" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O2"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -2591,22 +2616,815 @@
       <c r="N3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="O3" s="42" t="s">
         <v>86</v>
       </c>
+      <c r="P3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="R3" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="S3" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="T3" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="U3" s="42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="M4">
+        <v>13</v>
+      </c>
+      <c r="N4">
+        <v>14</v>
+      </c>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O26"/>
+    </row>
+    <row r="27" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O27"/>
+    </row>
+    <row r="28" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O28"/>
+    </row>
+    <row r="29" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O31"/>
+    </row>
+    <row r="32" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O32"/>
+    </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34"/>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O35"/>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O37"/>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O38"/>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O39"/>
+    </row>
+    <row r="40" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O40"/>
+    </row>
+    <row r="41" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O41"/>
+    </row>
+    <row r="42" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O42"/>
+    </row>
+    <row r="43" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O44"/>
+    </row>
+    <row r="45" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O45"/>
+    </row>
+    <row r="46" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O46"/>
+    </row>
+    <row r="47" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O47"/>
+    </row>
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O50"/>
+    </row>
+    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O51"/>
+    </row>
+    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O52"/>
+    </row>
+    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O54"/>
+    </row>
+    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O56"/>
+    </row>
+    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O57"/>
+    </row>
+    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O58"/>
+    </row>
+    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O59"/>
+    </row>
+    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O60"/>
+    </row>
+    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O61"/>
+    </row>
+    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O62"/>
+    </row>
+    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O63"/>
+    </row>
+    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O64"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65"/>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66"/>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O67"/>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O68"/>
+    </row>
+    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O69"/>
+    </row>
+    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O70"/>
+    </row>
+    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O71"/>
+    </row>
+    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O72"/>
+    </row>
+    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O73"/>
+    </row>
+    <row r="74" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O74"/>
+    </row>
+    <row r="75" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O75"/>
+    </row>
+    <row r="76" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O76"/>
+    </row>
+    <row r="77" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O77"/>
+    </row>
+    <row r="78" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O78"/>
+    </row>
+    <row r="79" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O79"/>
+    </row>
+    <row r="80" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O80"/>
+    </row>
+    <row r="81" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O81"/>
+    </row>
+    <row r="82" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O82"/>
+    </row>
+    <row r="83" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O83"/>
+    </row>
+    <row r="84" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O84"/>
+    </row>
+    <row r="85" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O85"/>
+    </row>
+    <row r="86" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O86"/>
+    </row>
+    <row r="87" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O87"/>
+    </row>
+    <row r="88" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O88"/>
+    </row>
+    <row r="89" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O89"/>
+    </row>
+    <row r="90" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O90"/>
+    </row>
+    <row r="91" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O91"/>
+    </row>
+    <row r="92" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O92"/>
+    </row>
+    <row r="93" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O93"/>
+    </row>
+    <row r="94" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O94"/>
+    </row>
+    <row r="95" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O95"/>
+    </row>
+    <row r="96" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O96"/>
+    </row>
+    <row r="97" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O97"/>
+    </row>
+    <row r="98" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O98"/>
+    </row>
+    <row r="99" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O99"/>
+    </row>
+    <row r="100" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O100"/>
+    </row>
+    <row r="101" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O101"/>
+    </row>
+    <row r="102" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O102"/>
+    </row>
+    <row r="103" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O103"/>
+    </row>
+    <row r="104" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O104"/>
+    </row>
+    <row r="105" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O105"/>
+    </row>
+    <row r="106" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O106"/>
+    </row>
+    <row r="107" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O107"/>
+    </row>
+    <row r="108" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O108"/>
+    </row>
+    <row r="109" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O109"/>
+    </row>
+    <row r="110" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O110"/>
+    </row>
+    <row r="111" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O111"/>
+    </row>
+    <row r="112" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O112"/>
+    </row>
+    <row r="113" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O113"/>
+    </row>
+    <row r="114" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O114"/>
+    </row>
+    <row r="115" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O115"/>
+    </row>
+    <row r="116" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O116"/>
+    </row>
+    <row r="117" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O117"/>
+    </row>
+    <row r="118" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O118"/>
+    </row>
+    <row r="119" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O119"/>
+    </row>
+    <row r="120" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O120"/>
+    </row>
+    <row r="121" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O121"/>
+    </row>
+    <row r="122" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O122"/>
+    </row>
+    <row r="123" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O123"/>
+    </row>
+    <row r="124" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O124"/>
+    </row>
+    <row r="125" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O125"/>
+    </row>
+    <row r="126" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O126"/>
+    </row>
+    <row r="127" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O127"/>
+    </row>
+    <row r="128" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O128"/>
+    </row>
+    <row r="129" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O129"/>
+    </row>
+    <row r="130" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O130"/>
+    </row>
+    <row r="131" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O131"/>
+    </row>
+    <row r="132" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O132"/>
+    </row>
+    <row r="133" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O133"/>
+    </row>
+    <row r="134" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O134"/>
+    </row>
+    <row r="135" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O135"/>
+    </row>
+    <row r="136" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O136"/>
+    </row>
+    <row r="137" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O137"/>
+    </row>
+    <row r="138" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O138"/>
+    </row>
+    <row r="139" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O139"/>
+    </row>
+    <row r="140" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O140"/>
+    </row>
+    <row r="141" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O141"/>
+    </row>
+    <row r="142" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O142"/>
+    </row>
+    <row r="143" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O143"/>
+    </row>
+    <row r="144" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O144"/>
+    </row>
+    <row r="145" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O145"/>
+    </row>
+    <row r="146" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O146"/>
+    </row>
+    <row r="147" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O147"/>
+    </row>
+    <row r="148" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O148"/>
+    </row>
+    <row r="149" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O149"/>
+    </row>
+    <row r="150" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O150"/>
+    </row>
+    <row r="151" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O151"/>
+    </row>
+    <row r="152" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O152"/>
+    </row>
+    <row r="153" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O153"/>
+    </row>
+    <row r="154" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O154"/>
+    </row>
+    <row r="155" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O155"/>
+    </row>
+    <row r="156" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O156"/>
+    </row>
+    <row r="157" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O157"/>
+    </row>
+    <row r="158" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O158"/>
+    </row>
+    <row r="159" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O159"/>
+    </row>
+    <row r="160" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O160"/>
+    </row>
+    <row r="161" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O161"/>
+    </row>
+    <row r="162" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O162"/>
+    </row>
+    <row r="163" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O163"/>
+    </row>
+    <row r="164" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O164"/>
+    </row>
+    <row r="165" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O165"/>
+    </row>
+    <row r="166" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O166"/>
+    </row>
+    <row r="167" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O167"/>
+    </row>
+    <row r="168" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O168"/>
+    </row>
+    <row r="169" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O169"/>
+    </row>
+    <row r="170" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O170"/>
+    </row>
+    <row r="171" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O171"/>
+    </row>
+    <row r="172" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O172"/>
+    </row>
+    <row r="173" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O173"/>
+    </row>
+    <row r="174" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O174"/>
+    </row>
+    <row r="175" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O175"/>
+    </row>
+    <row r="176" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O176"/>
+    </row>
+    <row r="177" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O177"/>
+    </row>
+    <row r="178" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O178"/>
+    </row>
+    <row r="179" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O179"/>
+    </row>
+    <row r="180" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O180"/>
+    </row>
+    <row r="181" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O181"/>
+    </row>
+    <row r="182" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O182"/>
+    </row>
+    <row r="183" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O183"/>
+    </row>
+    <row r="184" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O184"/>
+    </row>
+    <row r="185" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O185"/>
+    </row>
+    <row r="186" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O186"/>
+    </row>
+    <row r="187" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O187"/>
+    </row>
+    <row r="188" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O188"/>
+    </row>
+    <row r="189" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O189"/>
+    </row>
+    <row r="190" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O190"/>
+    </row>
+    <row r="191" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O191"/>
+    </row>
+    <row r="192" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O192"/>
+    </row>
+    <row r="193" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O193"/>
+    </row>
+    <row r="194" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O194"/>
+    </row>
+    <row r="195" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O195"/>
+    </row>
+    <row r="196" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O196"/>
+    </row>
+    <row r="197" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O197"/>
+    </row>
+    <row r="198" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O198"/>
+    </row>
+    <row r="199" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O199"/>
+    </row>
+    <row r="200" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O200"/>
+    </row>
+    <row r="201" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O201"/>
+    </row>
+    <row r="202" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O202"/>
+    </row>
+    <row r="203" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O203"/>
+    </row>
+    <row r="204" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O204"/>
+    </row>
+    <row r="205" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O205"/>
+    </row>
+    <row r="206" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O206"/>
+    </row>
+    <row r="207" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O207"/>
+    </row>
+    <row r="208" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O208"/>
+    </row>
+    <row r="209" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O209"/>
+    </row>
+    <row r="210" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O210"/>
+    </row>
+    <row r="211" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O211"/>
+    </row>
+    <row r="212" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O212"/>
+    </row>
+    <row r="213" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O213"/>
+    </row>
+    <row r="214" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O214"/>
+    </row>
+    <row r="215" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O215"/>
+    </row>
+    <row r="216" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O216"/>
+    </row>
+    <row r="217" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O217"/>
+    </row>
+    <row r="218" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O218"/>
+    </row>
+    <row r="219" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O219"/>
+    </row>
+    <row r="220" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O220"/>
+    </row>
+    <row r="221" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O221"/>
+    </row>
+    <row r="222" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O222"/>
+    </row>
+    <row r="223" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O223"/>
+    </row>
+    <row r="224" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O224"/>
+    </row>
+    <row r="225" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O225"/>
+    </row>
+    <row r="226" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O226"/>
+    </row>
+    <row r="227" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O227"/>
+    </row>
+    <row r="228" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O228"/>
+    </row>
+    <row r="229" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O229"/>
+    </row>
+    <row r="230" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O230"/>
+    </row>
+    <row r="231" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O231"/>
+    </row>
+    <row r="232" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O232"/>
+    </row>
+    <row r="233" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O233"/>
+    </row>
+    <row r="234" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O234"/>
+    </row>
+    <row r="235" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O235"/>
+    </row>
+    <row r="236" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O236"/>
+    </row>
+    <row r="237" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O237"/>
+    </row>
+    <row r="238" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O238"/>
+    </row>
+    <row r="239" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O239"/>
+    </row>
+    <row r="240" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O240"/>
+    </row>
+    <row r="241" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O241"/>
+    </row>
+    <row r="242" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O242"/>
+    </row>
+    <row r="243" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O243"/>
+    </row>
+    <row r="244" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O244"/>
+    </row>
+    <row r="245" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O245"/>
+    </row>
+    <row r="246" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O246"/>
+    </row>
+    <row r="247" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O247"/>
+    </row>
+    <row r="248" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O248"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="J2"/>
-    <mergeCell ref="K2"/>
-    <mergeCell ref="L2"/>
-    <mergeCell ref="M2"/>
-    <mergeCell ref="N2"/>
+  <mergeCells count="8">
     <mergeCell ref="C2"/>
     <mergeCell ref="D2"/>
     <mergeCell ref="G2"/>
     <mergeCell ref="H2"/>
     <mergeCell ref="I2"/>
+    <mergeCell ref="J2"/>
+    <mergeCell ref="K2"/>
+    <mergeCell ref="L2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2623,13 +3441,14 @@
       <selection activeCell="B44" sqref="B44"/>
       <selection pane="topRight" activeCell="B44" sqref="B44"/>
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD41"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>